<commit_message>
checkpoint - stitching together tract master dataset
</commit_message>
<xml_diff>
--- a/data/data-sources.xlsx
+++ b/data/data-sources.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="17600"/>
+    <workbookView windowWidth="18350" windowHeight="18320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -855,7 +855,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -886,6 +886,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1207,8 +1208,8 @@
   <sheetPr/>
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1428,7 +1429,7 @@
         <v>45999</v>
       </c>
       <c r="M5" s="5"/>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="12" t="s">
         <v>50</v>
       </c>
       <c r="O5" s="1"/>
@@ -1889,6 +1890,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1" display="https://data.cdc.gov/500-Cities-Places/PLACES-Census-Tract-Data-GIS-Friendly-Format-2025-/yjkw-uj5s/about_data"/>
+    <hyperlink ref="N5" r:id="rId2" display="https://download.geofabrik.de/north-america/us/new-york.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
wip: switching gears, saving progress on raster calculation
</commit_message>
<xml_diff>
--- a/data/data-sources.xlsx
+++ b/data/data-sources.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="18320"/>
+    <workbookView windowWidth="18350" windowHeight="10520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
   <si>
     <t>Dataset Name</t>
   </si>
@@ -202,10 +202,25 @@
     <t>filter: land cover, conus</t>
   </si>
   <si>
-    <t>Land Coverage by type (forest, opent water, etc)</t>
+    <t>Land Coverage by type (forest, opent water, etc) (30m resolution)</t>
   </si>
   <si>
     <t>https://www.mrlc.gov/data?f%5B0%5D=category%3ALand%20Cover&amp;f%5B1%5D=region%3Aconus</t>
+  </si>
+  <si>
+    <t>land_cover_nyc</t>
+  </si>
+  <si>
+    <t>Land_Cover</t>
+  </si>
+  <si>
+    <t>data/raw/land_cover/land_cover_nyc</t>
+  </si>
+  <si>
+    <t>Land Coverage NYC (6 in Resolution)</t>
+  </si>
+  <si>
+    <t>https://catalog.data.gov/dataset/land-cover-raster-data-2017-6in-resolution?utm_source=chatgpt.com</t>
   </si>
 </sst>
 </file>
@@ -886,7 +901,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1209,7 +1224,7 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1462,7 +1477,9 @@
       <c r="K6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L6" s="5"/>
+      <c r="L6" s="10">
+        <v>45999</v>
+      </c>
       <c r="M6" s="5">
         <v>2024</v>
       </c>
@@ -1471,9 +1488,16 @@
       </c>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="2:15">
-      <c r="B7" s="1"/>
-      <c r="C7" s="5"/>
+    <row r="7" spans="1:15">
+      <c r="A7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="1"/>
@@ -1481,10 +1505,18 @@
       <c r="H7" s="1"/>
       <c r="I7" s="5"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="1"/>
+      <c r="K7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L7" s="10">
+        <v>46010</v>
+      </c>
+      <c r="M7" s="5">
+        <v>2017</v>
+      </c>
+      <c r="N7" t="s">
+        <v>63</v>
+      </c>
       <c r="O7" s="1"/>
     </row>
     <row r="8" spans="2:15">

</xml_diff>

<commit_message>
modeling pipeline created and tested using current feature set
</commit_message>
<xml_diff>
--- a/data/data-sources.xlsx
+++ b/data/data-sources.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="10520"/>
+    <workbookView windowWidth="18350" windowHeight="17600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="70">
   <si>
     <t>Dataset Name</t>
   </si>
@@ -221,6 +221,24 @@
   </si>
   <si>
     <t>https://catalog.data.gov/dataset/land-cover-raster-data-2017-6in-resolution?utm_source=chatgpt.com</t>
+  </si>
+  <si>
+    <t>nyc_boroughs</t>
+  </si>
+  <si>
+    <t>nybbwi_25d</t>
+  </si>
+  <si>
+    <t>data/raw/nyc_boroughs/</t>
+  </si>
+  <si>
+    <t>NYC Gov</t>
+  </si>
+  <si>
+    <t>NYC Borough Boundaries</t>
+  </si>
+  <si>
+    <t>https://www.nyc.gov/content/planning/pages/resources/datasets/borough-boundaries</t>
   </si>
 </sst>
 </file>
@@ -870,7 +888,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -901,7 +919,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1223,8 +1240,8 @@
   <sheetPr/>
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1444,7 +1461,7 @@
         <v>45999</v>
       </c>
       <c r="M5" s="5"/>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="9" t="s">
         <v>50</v>
       </c>
       <c r="O5" s="1"/>
@@ -1519,20 +1536,41 @@
       </c>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="2:15">
-      <c r="B8" s="1"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+    <row r="8" spans="1:15">
+      <c r="A8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="5"/>
+      <c r="G8" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="5"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="1"/>
+      <c r="K8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L8" s="10">
+        <v>46014</v>
+      </c>
+      <c r="M8" s="5">
+        <v>2025</v>
+      </c>
+      <c r="N8" t="s">
+        <v>69</v>
+      </c>
       <c r="O8" s="1"/>
     </row>
     <row r="9" spans="2:15">

</xml_diff>

<commit_message>
wip: built econ mobility model - first pass
</commit_message>
<xml_diff>
--- a/data/data-sources.xlsx
+++ b/data/data-sources.xlsx
@@ -157,7 +157,7 @@
     <t xml:space="preserve">economic outcomes by neighborhood </t>
   </si>
   <si>
-    <t>https://www.opportunityatlas.org/</t>
+    <t>https://opportunityinsights.org/data/?geographic_level=0&amp;topic=0&amp;paper_id=1652#resource-listing</t>
   </si>
   <si>
     <t>osm_ny_shp</t>
@@ -1240,8 +1240,8 @@
   <sheetPr/>
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1424,7 +1424,7 @@
         <v>45999</v>
       </c>
       <c r="M4" s="5"/>
-      <c r="N4" s="1" t="s">
+      <c r="N4" t="s">
         <v>42</v>
       </c>
       <c r="O4" s="1"/>

</xml_diff>